<commit_message>
Tidsregistering samt review af testsuite OC2
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Laura Poyner.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Laura Poyner.xlsx
@@ -17,6 +17,7 @@
     <definedName name="GyldigeRoller">'Gyldige roller'!$A$1:$A$30</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -278,6 +279,33 @@
   </si>
   <si>
     <t>SD og DCD for OC4</t>
+  </si>
+  <si>
+    <t>Testsuite OC1</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>SD for OC1</t>
+  </si>
+  <si>
+    <t>45min</t>
+  </si>
+  <si>
+    <t>SD fir OC1</t>
+  </si>
+  <si>
+    <t>1t 15m</t>
+  </si>
+  <si>
+    <t>DCD for OC1</t>
+  </si>
+  <si>
+    <t>40m</t>
+  </si>
+  <si>
+    <t>Testsuite OC2</t>
   </si>
 </sst>
 </file>
@@ -641,7 +669,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -649,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="A1:I23"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +695,7 @@
     <col min="11" max="11" width="31.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>54</v>
       </c>
@@ -680,7 +708,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1092,6 +1120,89 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.46875</v>
+      </c>
+      <c r="I24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.46875</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="I26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="I27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>92</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="I28" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1145,17 +1256,17 @@
     <col min="1" max="1" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1170,12 +1281,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1185,42 +1296,42 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1243,97 +1354,97 @@
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Review af UC + tidsregistering
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Laura Poyner.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Laura Poyner.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>UC8</t>
+  </si>
+  <si>
+    <t>UC3</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,6 +1308,29 @@
       </c>
       <c r="G37" s="5">
         <v>0.53125</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="I38" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidsreg. for fjerde gang i dag. (Og sidste, undskyld)
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Laura Poyner.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Laura Poyner.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>UC3</t>
+  </si>
+  <si>
+    <t>Review kode til OC1</t>
+  </si>
+  <si>
+    <t>Review kode til OC2</t>
   </si>
 </sst>
 </file>
@@ -686,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -694,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,6 +1337,40 @@
       </c>
       <c r="I38" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="I39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>100</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I40" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review/rettelser af SD7 - Tidsreg.
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Laura Poyner.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering - Laura Poyner.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -329,6 +329,30 @@
   </si>
   <si>
     <t>Review kode til OC2</t>
+  </si>
+  <si>
+    <t>Review SDD til UC7</t>
+  </si>
+  <si>
+    <t>Design UC7 om</t>
+  </si>
+  <si>
+    <t>15m</t>
+  </si>
+  <si>
+    <t>Testsuite for OC5</t>
+  </si>
+  <si>
+    <t>Testsuite for OC7 - not possible</t>
+  </si>
+  <si>
+    <t>2t 15m</t>
+  </si>
+  <si>
+    <t>OC5 - Not possible - Design omarbejdes</t>
+  </si>
+  <si>
+    <t>OC7</t>
   </si>
 </sst>
 </file>
@@ -700,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,12 +1397,112 @@
         <v>64</v>
       </c>
     </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>42809</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0.40625</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" t="s">
+        <v>102</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>104</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0.53125</v>
+      </c>
+      <c r="I44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>105</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0.53125</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0.59722222222222221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>108</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0.60069444444444442</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E109">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E110">
       <formula1>GyldigeRoller</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">

</xml_diff>